<commit_message>
refactor to allow writing excel in chunks
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/expected/seqRepRows.xlsx
+++ b/src/test/resources/excel/expected/seqRepRows.xlsx
@@ -102,9 +102,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
+      <xdr:colOff>784080</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
+      <xdr:rowOff>92160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -122,197 +122,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
+          <a:ext cx="1269840" cy="1407360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -482,11 +292,6 @@
         <v>10.0</v>
       </c>
     </row>
-    <row r="23">
-</row>
-    <row r="24" customHeight="true" ht="12.8">
-      <c r="A24" s="2"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
AppendOnlyWriter Exscalabur Integration (#25)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/expected/seqRepRows.xlsx
+++ b/src/test/resources/excel/expected/seqRepRows.xlsx
@@ -131,196 +131,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>581040</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>208800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>784800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>92880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="581040" y="208800"/>
-          <a:ext cx="1270560" cy="1408080"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -482,11 +292,6 @@
         <v>10.0</v>
       </c>
     </row>
-    <row r="23">
-</row>
-    <row r="24" customHeight="true" ht="12.8">
-      <c r="A24" s="2"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>

</xml_diff>